<commit_message>
Backlog file was updated
</commit_message>
<xml_diff>
--- a/src/Codecool Shop _ Product Backlog.xlsx
+++ b/src/Codecool Shop _ Product Backlog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -304,6 +304,7 @@
       <color rgb="FF0000FF"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -503,7 +504,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -706,11 +707,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="41500425"/>
-        <c:axId val="72049328"/>
+        <c:axId val="16774943"/>
+        <c:axId val="94507885"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="41500425"/>
+        <c:axId val="16774943"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,14 +740,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72049328"/>
+        <c:crossAx val="94507885"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72049328"/>
+        <c:axId val="94507885"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -784,7 +785,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41500425"/>
+        <c:crossAx val="16774943"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -845,9 +846,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>208440</xdr:colOff>
+      <xdr:colOff>208080</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>98640</xdr:rowOff>
+      <xdr:rowOff>98280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -856,7 +857,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="8627040" cy="6275880"/>
+        <a:ext cx="8635680" cy="6275520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -879,10 +880,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.29"/>
@@ -997,7 +998,9 @@
         <v>200</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="H5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11057,7 +11060,7 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52.43"/>
   </cols>
@@ -14221,7 +14224,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>